<commit_message>
Added author names, checks, and styling adjustments.
Refined the project by adding author names, implementing crucial checks, and enhancing styling for better presentation.
</commit_message>
<xml_diff>
--- a/TrashItTestCases.xlsx
+++ b/TrashItTestCases.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philip James\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78B3042-7966-4710-A657-7846179E7301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2F6DB97B-2025-435D-B00B-41792D53504C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Case" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Prototype" sheetId="2" r:id="rId1"/>
+    <sheet name="Final" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="75">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -277,12 +276,79 @@
   <si>
     <t>User receives a confirmation message: "Payment successful."</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Navigate to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Payment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pay Now</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button.</t>
+    </r>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comments/Remarks</t>
+  </si>
+  <si>
+    <t>Philip James Olbedencia</t>
+  </si>
+  <si>
+    <t>Ryu R. Mendoza</t>
+  </si>
+  <si>
+    <t>TrashIt Test Cases</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,16 +371,99 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Segoe UI Historic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Segoe UI Historic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="48"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -322,11 +471,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -334,9 +527,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -355,16 +581,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>704851</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>172539</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>896471</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2855901</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>111579</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -379,8 +605,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="419100" y="202154"/>
-          <a:ext cx="2790265" cy="4432599"/>
+          <a:off x="5127172" y="172539"/>
+          <a:ext cx="2151050" cy="4701540"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -561,16 +787,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1725707</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>296958</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>176605</xdr:rowOff>
+      <xdr:rowOff>122176</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1774372</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3094265</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>126851</xdr:rowOff>
+      <xdr:rowOff>72422</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -585,8 +811,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4033478" y="176605"/>
-          <a:ext cx="3009580" cy="4576675"/>
+          <a:off x="8338779" y="122176"/>
+          <a:ext cx="2797307" cy="4712746"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -934,6 +1160,10 @@
             <a:rPr lang="en-PH" b="1"/>
             <a:t>Actual Results:</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-PH"/>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-PH"/>
           </a:br>
@@ -950,6 +1180,10 @@
           <a:r>
             <a:rPr lang="en-PH" b="1"/>
             <a:t>Comments:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH"/>
+            <a:t/>
           </a:r>
           <a:br>
             <a:rPr lang="en-PH"/>
@@ -1139,6 +1373,10 @@
             <a:rPr lang="en-PH" i="1"/>
             <a:t>(To be filled during testing)</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-PH"/>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-PH"/>
           </a:br>
@@ -1314,6 +1552,10 @@
             <a:rPr lang="en-PH" b="1"/>
             <a:t>Actual Results:</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-PH"/>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-PH"/>
           </a:br>
@@ -1329,12 +1571,20 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-PH"/>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-PH"/>
           </a:br>
           <a:r>
             <a:rPr lang="en-PH" b="1"/>
             <a:t>Comments:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH"/>
+            <a:t/>
           </a:r>
           <a:br>
             <a:rPr lang="en-PH"/>
@@ -1688,14 +1938,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>102891</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>175873</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>456549</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>166842</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3656949</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>230342</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1732,14 +1982,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>107577</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>386671</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>107576</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3587071</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171076</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1776,14 +2026,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>75210</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>26721</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>551807</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>86696</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3752207</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>162896</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1820,14 +2070,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>62098</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>156852</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>11875</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>156852</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3821875</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>169552</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1864,14 +2114,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2284019</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>166254</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>91294</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>149431</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3901294</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>174831</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1906,16 +2156,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2286993</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>29568</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>162298</xdr:rowOff>
+      <xdr:rowOff>9898</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>109848</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>49638</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4025900</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>182374</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1938,8 +2188,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15310266" y="14931243"/>
-          <a:ext cx="3988128" cy="2588977"/>
+          <a:off x="15371168" y="23619198"/>
+          <a:ext cx="3996332" cy="2801376"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1954,7 +2204,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Slidehelper - 024">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1962,34 +2212,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="323232"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E3DED1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="0E103D"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="69306D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="A5668B"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="D3BCC0"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="F2D7EE"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="BFBFBF"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="F2D7EE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="D3BCC0"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -2247,23 +2497,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FA0802-828B-4A26-BD4D-88D47E7280D9}">
-  <dimension ref="B56:H140"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H140"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:N151"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="41.33203125" customWidth="1"/>
-    <col min="4" max="4" width="54.33203125" customWidth="1"/>
-    <col min="5" max="5" width="64.33203125" customWidth="1"/>
-    <col min="6" max="6" width="99.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
+    <col min="4" max="4" width="54.28515625" customWidth="1"/>
+    <col min="5" max="5" width="64.28515625" customWidth="1"/>
+    <col min="6" max="6" width="99.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.5">
+      <c r="A3" s="14"/>
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="1:2" ht="25.5" x14ac:dyDescent="0.5">
+      <c r="A4" s="14"/>
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:2" ht="25.5" x14ac:dyDescent="0.5">
+      <c r="A5" s="14"/>
+      <c r="B5" s="12"/>
+    </row>
+    <row r="6" spans="1:2" ht="25.5" x14ac:dyDescent="0.5">
+      <c r="A6" s="14"/>
+      <c r="B6" s="12"/>
+    </row>
+    <row r="7" spans="1:2" ht="25.5" x14ac:dyDescent="0.5">
+      <c r="A7" s="14"/>
+      <c r="B7" s="12"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
         <v>0</v>
       </c>
@@ -2283,7 +2566,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>1</v>
       </c>
@@ -2300,7 +2583,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D58" s="1" t="s">
         <v>6</v>
       </c>
@@ -2311,7 +2594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E59" s="1" t="s">
         <v>10</v>
       </c>
@@ -2319,17 +2602,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E60" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E61" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>18</v>
       </c>
@@ -2346,7 +2629,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D73" s="1" t="s">
         <v>21</v>
       </c>
@@ -2357,7 +2640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E74" s="1" t="s">
         <v>24</v>
       </c>
@@ -2365,12 +2648,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E75" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
         <v>29</v>
       </c>
@@ -2387,7 +2670,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D88" s="3" t="s">
         <v>32</v>
       </c>
@@ -2398,7 +2681,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E89" s="4" t="s">
         <v>38</v>
       </c>
@@ -2406,10 +2689,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E90" s="4"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
         <v>34</v>
       </c>
@@ -2426,7 +2709,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D105" s="1" t="s">
         <v>31</v>
       </c>
@@ -2437,7 +2720,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E106" s="1" t="s">
         <v>46</v>
       </c>
@@ -2445,12 +2728,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E107" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="1" t="s">
         <v>35</v>
       </c>
@@ -2467,7 +2750,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D120" s="4" t="s">
         <v>53</v>
       </c>
@@ -2475,7 +2758,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
         <v>36</v>
       </c>
@@ -2492,7 +2775,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D137" t="s">
         <v>58</v>
       </c>
@@ -2503,7 +2786,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
         <v>59</v>
       </c>
@@ -2514,12 +2797,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E139" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E140" t="s">
         <v>63</v>
       </c>
@@ -2532,286 +2815,328 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AFB342-8787-43B4-A34E-37A60F6F93B9}">
-  <dimension ref="A2:G86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" customWidth="1"/>
-    <col min="4" max="4" width="65.88671875" customWidth="1"/>
-    <col min="5" max="5" width="58.109375" customWidth="1"/>
-    <col min="6" max="6" width="33.5546875" customWidth="1"/>
-    <col min="7" max="7" width="29.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="65.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="58.140625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" customWidth="1"/>
+    <col min="8" max="8" width="37.5703125" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="H3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
+    <row r="5" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="C5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D5" s="1" t="s">
+    <row r="6" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="D6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D6" s="1" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D7" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D7" s="1" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D8" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="1" t="s">
+    <row r="20" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="C20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D20" s="1" t="s">
+    <row r="21" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="D21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D21" s="1" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D22" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D34" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E34" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C34" s="3" t="s">
+    <row r="35" spans="1:5" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="C35" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D35" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E35" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D35" s="4" t="s">
+    <row r="36" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="D36" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E36" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D36" s="4"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D37" s="11"/>
+    </row>
+    <row r="51" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D51" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C51" s="1" t="s">
+    <row r="52" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="C52" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E52" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D52" s="1" t="s">
+    <row r="53" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="D53" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E53" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D53" s="1" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D54" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:5" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A66" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C66" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D66" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E66" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C66" s="4" t="s">
+    <row r="67" spans="1:5" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="C67" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D67" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:5" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A83" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D82" t="s">
-        <v>60</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="D83" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E83" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C83" t="s">
+    <row r="84" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="C84" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D84" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E84" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C84" t="s">
+    <row r="85" spans="1:5" ht="75" x14ac:dyDescent="0.3">
+      <c r="C85" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D85" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E85" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D85" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D86" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D86" t="s">
-        <v>63</v>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D87" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D1:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>